<commit_message>
Conrad - single quote for Voltcraft Power supply added
</commit_message>
<xml_diff>
--- a/Budget KIIWI Projekt V4 - 01.xlsx
+++ b/Budget KIIWI Projekt V4 - 01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Material" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="153">
   <si>
     <t>Number of 
 devices (part)</t>
@@ -609,6 +609,12 @@
   </si>
   <si>
     <t>Nohau-Joulescope.pdf</t>
+  </si>
+  <si>
+    <t>Cornad</t>
+  </si>
+  <si>
+    <t>Conrad-Voltcraft-PS.pdf</t>
   </si>
 </sst>
 </file>
@@ -811,7 +817,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
@@ -1108,6 +1114,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1376,11 +1385,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z32"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="J6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="N6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P7" sqref="P7"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1411,26 +1420,26 @@
       <c r="D1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="111" t="s">
+      <c r="E1" s="112" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="111"/>
-      <c r="G1" s="111"/>
-      <c r="H1" s="111"/>
-      <c r="I1" s="111" t="s">
+      <c r="F1" s="112"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="112"/>
+      <c r="I1" s="112" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="111"/>
-      <c r="K1" s="111"/>
-      <c r="L1" s="111"/>
-      <c r="M1" s="111" t="s">
+      <c r="J1" s="112"/>
+      <c r="K1" s="112"/>
+      <c r="L1" s="112"/>
+      <c r="M1" s="112" t="s">
         <v>36</v>
       </c>
-      <c r="N1" s="111"/>
-      <c r="O1" s="111" t="s">
+      <c r="N1" s="112"/>
+      <c r="O1" s="112" t="s">
         <v>40</v>
       </c>
-      <c r="P1" s="111"/>
+      <c r="P1" s="112"/>
       <c r="Q1" s="7" t="s">
         <v>18</v>
       </c>
@@ -2639,10 +2648,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2654,7 +2663,7 @@
     <col min="10" max="10" width="11.75" style="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>37</v>
       </c>
@@ -2689,8 +2698,11 @@
       <c r="L1" s="108" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="111" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="54"/>
@@ -2699,7 +2711,7 @@
       <c r="G2" s="81"/>
       <c r="H2" s="78"/>
     </row>
-    <row r="3" spans="1:12" s="68" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="68" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
         <v>4</v>
       </c>
@@ -2730,7 +2742,7 @@
         <v>462.36</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="19">
         <v>6</v>
       </c>
@@ -2765,7 +2777,7 @@
         <v>3374.1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="68" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <v>7</v>
       </c>
@@ -2797,7 +2809,7 @@
         <v>1331.7</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="19">
         <v>8</v>
       </c>
@@ -2826,7 +2838,7 @@
       </c>
       <c r="J6" s="76"/>
     </row>
-    <row r="7" spans="1:12" s="68" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
         <v>9</v>
       </c>
@@ -2858,7 +2870,7 @@
         <v>4745.46</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="69" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="69" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
         <v>11</v>
       </c>
@@ -2882,12 +2894,15 @@
         <f t="shared" si="0"/>
         <v>918</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I8" s="94">
         <v>411.48</v>
       </c>
       <c r="J8" s="76"/>
-    </row>
-    <row r="9" spans="1:12" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M8" s="94">
+        <v>397.04</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>13</v>
       </c>
@@ -2918,7 +2933,7 @@
         <v>142.5</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="104" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" s="104" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="101">
         <v>10</v>
       </c>
@@ -2941,7 +2956,7 @@
         <v>979.02</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="92" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="92" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="92" t="s">
         <v>118</v>
       </c>
@@ -2956,7 +2971,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>112</v>
       </c>
@@ -2975,8 +2990,11 @@
       <c r="L12">
         <v>10430.18</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <v>397.04</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>113</v>
       </c>
@@ -2993,8 +3011,11 @@
       <c r="L13">
         <v>1981.73</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <v>75.44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>114</v>
       </c>
@@ -3005,7 +3026,7 @@
       <c r="E14" s="91">
         <v>13729.74</v>
       </c>
-      <c r="I14" s="91">
+      <c r="I14" s="19">
         <v>19589.099999999999</v>
       </c>
       <c r="J14" s="48">
@@ -3017,8 +3038,11 @@
       <c r="L14">
         <v>12411.91</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" s="98" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M14" s="109">
+        <v>472.48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="98" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="98" t="s">
         <v>119</v>
       </c>
@@ -3034,7 +3058,7 @@
       </c>
       <c r="J16" s="100"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>120</v>
       </c>
@@ -3051,12 +3075,17 @@
         <v>141</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L18" s="50" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M20" s="50" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="97"/>
       <c r="B22" s="106" t="s">
         <v>136</v>
@@ -3086,9 +3115,10 @@
     <hyperlink ref="K22" r:id="rId5"/>
     <hyperlink ref="K17" r:id="rId6"/>
     <hyperlink ref="L18" r:id="rId7"/>
+    <hyperlink ref="M20" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -3096,7 +3126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>

</xml_diff>